<commit_message>
thresholds updated and temperature interpolation added
</commit_message>
<xml_diff>
--- a/documentation/temp sensor calculator.xlsx
+++ b/documentation/temp sensor calculator.xlsx
@@ -2,30 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loz\SkyDrive\documents\amateur radio\SDR\amplifier protection\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loz\SkyDrive\documents\amateur radio\SDR\ganymede\github\Ganymede\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="temp sensor" sheetId="1" r:id="rId1"/>
-    <sheet name="thresholds" sheetId="2" r:id="rId2"/>
+    <sheet name="voltage" sheetId="3" r:id="rId2"/>
+    <sheet name="Fwd, Reverse power" sheetId="4" r:id="rId3"/>
+    <sheet name="Current" sheetId="5" r:id="rId4"/>
+    <sheet name="comparator thresholds" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
   <si>
     <t>500W amplifier current sensing</t>
   </si>
@@ -106,50 +117,251 @@
     <t>current</t>
   </si>
   <si>
-    <t>fwd, rev power</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>assume full scale=120C, 0v = 0C</t>
-  </si>
-  <si>
-    <t>temp scale</t>
-  </si>
-  <si>
-    <t>20A full scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current scale </t>
-  </si>
-  <si>
-    <t>60V full scale</t>
-  </si>
-  <si>
-    <t>voltage scale</t>
-  </si>
-  <si>
-    <t>full scale power</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
-    <t>V full power</t>
-  </si>
-  <si>
-    <t>V scale = 200V</t>
-  </si>
-  <si>
-    <t>V scale for ADC</t>
+    <t>Input voltage</t>
+  </si>
+  <si>
+    <t>sensor voltage</t>
+  </si>
+  <si>
+    <t>AREF</t>
+  </si>
+  <si>
+    <t>ADC reading</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>Divider on pallet PCB:</t>
+  </si>
+  <si>
+    <t>* ADC reading</t>
+  </si>
+  <si>
+    <t>PSU Vin (V) =</t>
+  </si>
+  <si>
+    <t>scaling factor to convert ADC reading to PSU voltage:</t>
+  </si>
+  <si>
+    <t>PSU Voltage measurement scaling</t>
+  </si>
+  <si>
+    <t>Forward and reverse power</t>
+  </si>
+  <si>
+    <t>ADC count</t>
+  </si>
+  <si>
+    <t>(10 bits)</t>
+  </si>
+  <si>
+    <t>Arduino ADC count</t>
+  </si>
+  <si>
+    <t>Full scale voltage</t>
+  </si>
+  <si>
+    <t>R49, R50 on divider adjusted to give 5V for input power &gt; 500W</t>
+  </si>
+  <si>
+    <t>Full power calibrated value</t>
+  </si>
+  <si>
+    <t>we don't know the calibration of the VSWR bridge exactly</t>
+  </si>
+  <si>
+    <r>
+      <t>power = K. V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/R</t>
+    </r>
+  </si>
+  <si>
+    <t>R=50 ohms</t>
+  </si>
+  <si>
+    <t>K=</t>
+  </si>
+  <si>
+    <t>Calibration for power from ADC value:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power (W) = </t>
+  </si>
+  <si>
+    <r>
+      <t>* ADC reading</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Current Sensor</t>
+  </si>
+  <si>
+    <t>Output voltage scale</t>
+  </si>
+  <si>
+    <t>mV/A</t>
+  </si>
+  <si>
+    <t>full scale current</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino ADC full scale </t>
+  </si>
+  <si>
+    <t>Arduino ADC full count</t>
+  </si>
+  <si>
+    <t>Interpol</t>
+  </si>
+  <si>
+    <t>Hall effect sensor ACS723-40A</t>
+  </si>
+  <si>
+    <t>-40A assumed!</t>
+  </si>
+  <si>
+    <t>sensor circuit gain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anode current (A) = </t>
+  </si>
+  <si>
+    <t>effective scale</t>
+  </si>
+  <si>
+    <t>V/A</t>
+  </si>
+  <si>
+    <t>DAC output level</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>DAC full scale count</t>
+  </si>
+  <si>
+    <t>(8 bits)</t>
+  </si>
+  <si>
+    <t>trip voltage</t>
+  </si>
+  <si>
+    <t>DAC setting</t>
+  </si>
+  <si>
+    <t>trip current</t>
+  </si>
+  <si>
+    <t>reverse power</t>
+  </si>
+  <si>
+    <t>trip power</t>
+  </si>
+  <si>
+    <t>comparator voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor &amp; comparator input = </t>
+  </si>
+  <si>
+    <t>*input voltage</t>
+  </si>
+  <si>
+    <t>*power</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <t>Forward power trip</t>
+  </si>
+  <si>
+    <t>temperature trip</t>
+  </si>
+  <si>
+    <t>C (software)</t>
+  </si>
+  <si>
+    <t>W (software)</t>
+  </si>
+  <si>
+    <t>Full scale reading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +379,29 @@
     </font>
     <font>
       <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -231,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -243,6 +478,14 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,7 +518,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -331,7 +573,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'temp sensor'!$A$23:$A$43</c:f>
+              <c:f>'temp sensor'!$A$25:$A$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -403,7 +645,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'temp sensor'!$D$23:$D$43</c:f>
+              <c:f>'temp sensor'!$D$25:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -474,6 +716,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-145C-464F-9456-78D9F4972EA5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -484,9 +731,9 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="787363200"/>
-        <c:axId val="787360480"/>
-        <c:extLst>
+        <c:axId val="-1617135856"/>
+        <c:axId val="-1617135312"/>
+        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -506,10 +753,10 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'temp sensor'!$A$23:$A$43</c15:sqref>
+                          <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -584,10 +831,10 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'temp sensor'!$B$23:$B$43</c15:sqref>
+                          <c15:sqref>'temp sensor'!$B$25:$B$45</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -661,6 +908,11 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-145C-464F-9456-78D9F4972EA5}"/>
+                  </c:ext>
+                </c:extLst>
               </c15:ser>
             </c15:filteredLineSeries>
             <c15:filteredLineSeries>
@@ -681,10 +933,10 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'temp sensor'!$A$23:$A$43</c15:sqref>
+                          <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -759,10 +1011,10 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'temp sensor'!$C$23:$C$43</c15:sqref>
+                          <c15:sqref>'temp sensor'!$C$25:$C$45</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -836,6 +1088,11 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-145C-464F-9456-78D9F4972EA5}"/>
+                  </c:ext>
+                </c:extLst>
               </c15:ser>
             </c15:filteredLineSeries>
             <c15:filteredLineSeries>
@@ -856,10 +1113,10 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'temp sensor'!$A$23:$A$43</c15:sqref>
+                          <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -934,10 +1191,10 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'temp sensor'!$D$23:$D$43</c15:sqref>
+                          <c15:sqref>'temp sensor'!$D$25:$D$45</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1011,13 +1268,18 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-145C-464F-9456-78D9F4972EA5}"/>
+                  </c:ext>
+                </c:extLst>
               </c15:ser>
             </c15:filteredLineSeries>
           </c:ext>
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="787363200"/>
+        <c:axId val="-1617135856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1054,7 +1316,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1121,7 +1382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="787360480"/>
+        <c:crossAx val="-1617135312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1129,7 +1390,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="787360480"/>
+        <c:axId val="-1617135312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1436,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1236,9 +1496,614 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="787363200"/>
+        <c:crossAx val="-1617135856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'temp sensor'!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Temp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'temp sensor'!$E$24:$E$57</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.645099959670446</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.772653458915229</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>123.47818319860657</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150.93350802489357</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>182.20640569395019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>217.70078740157481</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256.47495361781074</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>298.28460459596505</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>342.51734390485632</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>388.1238155401137</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>434.64864015091973</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>481.73122157754432</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>528.04675413968948</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>572.62390489406221</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>615.19291531307022</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>655.42991252400248</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>692.91496453722959</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>727.54065575496031</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>759.1871030454804</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>787.92576717887925</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>813.84190602904721</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>836.8114722591306</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>857.32093409779441</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>875.67660016532955</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>891.97742956417369</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>906.31648304098542</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>919.01450585685598</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>930.30767988371156</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>940.29942115537654</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>949.17348988104436</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>957.02590906730825</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>963.97304166826473</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>1023</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'temp sensor'!$A$24:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3B35-43A7-9D2C-73572078976D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'temp sensor'!$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Interpol</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'temp sensor'!$F$24:$F$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>693</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>906</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>949</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1023</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'temp sensor'!$G$24:$G$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3B35-43A7-9D2C-73572078976D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1617127696"/>
+        <c:axId val="-1617134768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1617127696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1617134768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1617134768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="180"/>
+          <c:min val="-20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1617127696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1281,8 +2146,15 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="span"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1357,6 +2229,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1854,6 +2766,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1890,7 +3318,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1934,7 +3368,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1978,7 +3418,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -2022,7 +3468,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvPr id="9" name="Straight Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -2061,12 +3513,18 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2076,6 +3534,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2347,10 +3841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView topLeftCell="F44" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51:G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,7 +3871,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
@@ -2421,7 +3915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>18</v>
       </c>
@@ -2432,7 +3926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -2446,7 +3940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>16</v>
       </c>
@@ -2457,441 +3951,762 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21">
+        <v>1024</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>13</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-20</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8">
+        <f>(D24/E$20)*E$21</f>
         <v>0</v>
       </c>
-      <c r="B23">
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
         <v>3.2014</v>
       </c>
-      <c r="C23">
-        <f>B23*$E$19</f>
+      <c r="C25">
+        <f>B25*$E$19</f>
         <v>32014</v>
       </c>
-      <c r="D23" s="7">
-        <f>$E$20*$E$18/($E$18+C23)</f>
+      <c r="D25" s="7">
+        <f>$E$20*$E$18/($E$18+C25)</f>
         <v>0.38889208964682837</v>
       </c>
-      <c r="E23" s="8">
-        <f>(D23/E$20)*1024</f>
+      <c r="E25" s="8">
+        <f>(D25/E$20)*E$21</f>
         <v>79.645099959670446</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>5</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>2.5011000000000001</v>
       </c>
-      <c r="C24">
-        <f t="shared" ref="C24:C43" si="0">B24*$E$19</f>
+      <c r="C26">
+        <f t="shared" ref="C26:C45" si="0">B26*$E$19</f>
         <v>25011</v>
       </c>
-      <c r="D24" s="7">
-        <f t="shared" ref="D24:D43" si="1">$E$20*$E$18/($E$18+C24)</f>
+      <c r="D26" s="7">
+        <f t="shared" ref="D26:D45" si="1">$E$20*$E$18/($E$18+C26)</f>
         <v>0.4871711594673595</v>
       </c>
-      <c r="E24" s="8">
-        <f t="shared" ref="E24:E43" si="2">(D24/E$20)*1024</f>
+      <c r="E26" s="8">
+        <f t="shared" ref="E26:E56" si="2">(D26/E$20)*E$21</f>
         <v>99.772653458915229</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="F26">
+        <v>100</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>10</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>1.9691000000000001</v>
       </c>
-      <c r="C25">
+      <c r="C27">
         <f t="shared" si="0"/>
         <v>19691</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D27" s="7">
         <f t="shared" si="1"/>
         <v>0.60292081639944617</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E27" s="8">
         <f t="shared" si="2"/>
         <v>123.47818319860657</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>15</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>1.5618000000000001</v>
       </c>
-      <c r="C26">
+      <c r="C28">
         <f t="shared" si="0"/>
         <v>15618</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D28" s="7">
         <f t="shared" si="1"/>
         <v>0.73698001965280058</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E28" s="8">
         <f t="shared" si="2"/>
         <v>150.93350802489357</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>20</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>1.2474000000000001</v>
       </c>
-      <c r="C27">
+      <c r="C29">
         <f t="shared" si="0"/>
         <v>12474</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D29" s="7">
         <f t="shared" si="1"/>
         <v>0.88967971530249113</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E29" s="8">
         <f t="shared" si="2"/>
         <v>182.20640569395019</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="F29">
+        <v>182</v>
+      </c>
+      <c r="G29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>25</v>
       </c>
-      <c r="B28">
+      <c r="B30">
         <v>1</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D30" s="7">
         <f t="shared" si="1"/>
         <v>1.0629921259842521</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E30" s="8">
         <f t="shared" si="2"/>
         <v>217.70078740157481</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B29">
+      <c r="B31">
         <v>0.80800000000000005</v>
       </c>
-      <c r="C29">
+      <c r="C31">
         <f t="shared" si="0"/>
         <v>8080.0000000000009</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D31" s="7">
         <f t="shared" si="1"/>
         <v>1.2523191094619666</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E31" s="8">
         <f t="shared" si="2"/>
         <v>256.47495361781074</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>35</v>
       </c>
-      <c r="B30">
+      <c r="B32">
         <v>0.65690000000000004</v>
       </c>
-      <c r="C30">
+      <c r="C32">
         <f t="shared" si="0"/>
         <v>6569</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D32" s="7">
         <f t="shared" si="1"/>
         <v>1.4564677958787355</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E32" s="8">
         <f t="shared" si="2"/>
         <v>298.28460459596505</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="F32">
+        <v>298</v>
+      </c>
+      <c r="G32">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>40</v>
       </c>
-      <c r="B31">
+      <c r="B33">
         <v>0.53720000000000001</v>
       </c>
-      <c r="C31">
+      <c r="C33">
         <f t="shared" si="0"/>
         <v>5372</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D33" s="7">
         <f t="shared" si="1"/>
         <v>1.6724479682854312</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E33" s="8">
         <f t="shared" si="2"/>
         <v>342.51734390485632</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>45</v>
       </c>
-      <c r="B32">
+      <c r="B34">
         <v>0.44235000000000002</v>
       </c>
-      <c r="C32">
+      <c r="C34">
         <f t="shared" si="0"/>
         <v>4423.5</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D34" s="7">
         <f t="shared" si="1"/>
         <v>1.8951358180669615</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E34" s="8">
         <f t="shared" si="2"/>
         <v>388.1238155401137</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>50</v>
       </c>
-      <c r="B33">
+      <c r="B35">
         <v>0.36609999999999998</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <f t="shared" si="0"/>
         <v>3661</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D35" s="7">
         <f t="shared" si="1"/>
         <v>2.1223078132369126</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E35" s="8">
         <f t="shared" si="2"/>
         <v>434.64864015091973</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="F35">
+        <v>435</v>
+      </c>
+      <c r="G35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>55</v>
       </c>
-      <c r="B34">
+      <c r="B36">
         <v>0.30392999999999998</v>
       </c>
-      <c r="C34">
+      <c r="C36">
         <f t="shared" si="0"/>
         <v>3039.2999999999997</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D36" s="7">
         <f t="shared" si="1"/>
         <v>2.3522032303591032</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E36" s="8">
         <f t="shared" si="2"/>
         <v>481.73122157754432</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>60</v>
       </c>
-      <c r="B35">
+      <c r="B37">
         <v>0.25358999999999998</v>
       </c>
-      <c r="C35">
+      <c r="C37">
         <f t="shared" si="0"/>
         <v>2535.8999999999996</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D37" s="7">
         <f t="shared" si="1"/>
         <v>2.5783532916977028</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E37" s="8">
         <f t="shared" si="2"/>
         <v>528.04675413968948</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>65</v>
       </c>
-      <c r="B36">
+      <c r="B38">
         <v>0.21282999999999999</v>
       </c>
-      <c r="C36">
+      <c r="C38">
         <f t="shared" si="0"/>
         <v>2128.2999999999997</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D38" s="7">
         <f t="shared" si="1"/>
         <v>2.7960151606155379</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E38" s="8">
         <f t="shared" si="2"/>
         <v>572.62390489406221</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="F38">
+        <v>573</v>
+      </c>
+      <c r="G38">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>70</v>
       </c>
-      <c r="B37">
+      <c r="B39">
         <v>0.17942</v>
       </c>
-      <c r="C37">
+      <c r="C39">
         <f t="shared" si="0"/>
         <v>1794.2</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D39" s="7">
         <f t="shared" si="1"/>
         <v>3.0038716568021004</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E39" s="8">
         <f t="shared" si="2"/>
         <v>615.19291531307022</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>75</v>
       </c>
-      <c r="B38">
+      <c r="B40">
         <v>0.15182999999999999</v>
       </c>
-      <c r="C38">
+      <c r="C40">
         <f t="shared" si="0"/>
         <v>1518.3</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D40" s="7">
         <f t="shared" si="1"/>
         <v>3.2003413697461061</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E40" s="8">
         <f t="shared" si="2"/>
         <v>655.42991252400248</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>80</v>
       </c>
-      <c r="B39">
+      <c r="B41">
         <v>0.12901000000000001</v>
       </c>
-      <c r="C39">
+      <c r="C41">
         <f t="shared" si="0"/>
         <v>1290.1000000000001</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D41" s="7">
         <f t="shared" si="1"/>
         <v>3.3833738502794413</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E41" s="8">
         <f t="shared" si="2"/>
         <v>692.91496453722959</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="F41">
+        <v>693</v>
+      </c>
+      <c r="G41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>85</v>
       </c>
-      <c r="B40">
+      <c r="B42">
         <v>0.11002000000000001</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <f t="shared" si="0"/>
         <v>1100.2</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D42" s="7">
         <f t="shared" si="1"/>
         <v>3.5524446081785173</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E42" s="8">
         <f t="shared" si="2"/>
         <v>727.54065575496031</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>90</v>
       </c>
-      <c r="B41">
+      <c r="B43">
         <v>9.4178999999999999E-2</v>
       </c>
-      <c r="C41">
+      <c r="C43">
         <f t="shared" si="0"/>
         <v>941.79</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D43" s="7">
         <f t="shared" si="1"/>
         <v>3.7069682765892598</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E43" s="8">
         <f t="shared" si="2"/>
         <v>759.1871030454804</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>95</v>
       </c>
-      <c r="B42">
+      <c r="B44">
         <v>8.0895999999999996E-2</v>
       </c>
-      <c r="C42">
+      <c r="C44">
         <f t="shared" si="0"/>
         <v>808.95999999999992</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D44" s="7">
         <f t="shared" si="1"/>
         <v>3.8472937850531213</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E44" s="8">
         <f t="shared" si="2"/>
         <v>787.92576717887925</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>100</v>
       </c>
-      <c r="B43">
+      <c r="B45">
         <v>6.9722000000000006E-2</v>
       </c>
-      <c r="C43">
+      <c r="C45">
         <f t="shared" si="0"/>
         <v>697.22</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D45" s="7">
         <f t="shared" si="1"/>
         <v>3.973837431782457</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E45" s="8">
         <f t="shared" si="2"/>
         <v>813.84190602904721</v>
+      </c>
+      <c r="F45">
+        <v>814</v>
+      </c>
+      <c r="G45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>105</v>
+      </c>
+      <c r="B46">
+        <v>6.0396999999999999E-2</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:C56" si="3">B46*$E$19</f>
+        <v>603.97</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" ref="D46:D56" si="4">$E$20*$E$18/($E$18+C46)</f>
+        <v>4.0859935168902863</v>
+      </c>
+      <c r="E46" s="8">
+        <f t="shared" si="2"/>
+        <v>836.8114722591306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>110</v>
+      </c>
+      <c r="B47">
+        <v>5.2492999999999998E-2</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="3"/>
+        <v>524.92999999999995</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="4"/>
+        <v>4.186137373524387</v>
+      </c>
+      <c r="E47" s="8">
+        <f t="shared" si="2"/>
+        <v>857.32093409779441</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>115</v>
+      </c>
+      <c r="B48">
+        <v>4.5733000000000003E-2</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="3"/>
+        <v>457.33000000000004</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="4"/>
+        <v>4.2757646492447732</v>
+      </c>
+      <c r="E48" s="8">
+        <f t="shared" si="2"/>
+        <v>875.67660016532955</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>120</v>
+      </c>
+      <c r="B49">
+        <v>3.9962999999999999E-2</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="3"/>
+        <v>399.63</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="4"/>
+        <v>4.3553585427938168</v>
+      </c>
+      <c r="E49" s="8">
+        <f t="shared" si="2"/>
+        <v>891.97742956417369</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>125</v>
+      </c>
+      <c r="B50">
+        <v>3.5059E-2</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="3"/>
+        <v>350.59</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="4"/>
+        <v>4.4253734523485617</v>
+      </c>
+      <c r="E50" s="8">
+        <f t="shared" si="2"/>
+        <v>906.31648304098542</v>
+      </c>
+      <c r="F50">
+        <v>906</v>
+      </c>
+      <c r="G50">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>130</v>
+      </c>
+      <c r="B51">
+        <v>3.0844E-2</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="3"/>
+        <v>308.44</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" si="4"/>
+        <v>4.4873755168791796</v>
+      </c>
+      <c r="E51" s="8">
+        <f t="shared" si="2"/>
+        <v>919.01450585685598</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>135</v>
+      </c>
+      <c r="B52">
+        <v>2.7192000000000001E-2</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="3"/>
+        <v>271.92</v>
+      </c>
+      <c r="D52" s="7">
+        <f t="shared" si="4"/>
+        <v>4.5425179681821852</v>
+      </c>
+      <c r="E52" s="8">
+        <f t="shared" si="2"/>
+        <v>930.30767988371156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>140</v>
+      </c>
+      <c r="B53">
+        <v>2.4034E-2</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="3"/>
+        <v>240.34</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" si="4"/>
+        <v>4.5913057673602369</v>
+      </c>
+      <c r="E53" s="8">
+        <f t="shared" si="2"/>
+        <v>940.29942115537654</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>145</v>
+      </c>
+      <c r="B54">
+        <v>2.1284999999999998E-2</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="3"/>
+        <v>212.85</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" si="4"/>
+        <v>4.6346361810597871</v>
+      </c>
+      <c r="E54" s="8">
+        <f t="shared" si="2"/>
+        <v>949.17348988104436</v>
+      </c>
+      <c r="F54">
+        <v>949</v>
+      </c>
+      <c r="G54">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>150</v>
+      </c>
+      <c r="B55">
+        <v>1.8894999999999999E-2</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="3"/>
+        <v>188.95</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="4"/>
+        <v>4.6729780716177158</v>
+      </c>
+      <c r="E55" s="8">
+        <f t="shared" si="2"/>
+        <v>957.02590906730825</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>155</v>
+      </c>
+      <c r="B56">
+        <v>1.6813000000000002E-2</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="3"/>
+        <v>168.13000000000002</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="4"/>
+        <v>4.7068996175208238</v>
+      </c>
+      <c r="E56" s="8">
+        <f t="shared" si="2"/>
+        <v>963.97304166826473</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>180</v>
+      </c>
+      <c r="E57">
+        <v>1023</v>
+      </c>
+      <c r="F57">
+        <v>1023</v>
+      </c>
+      <c r="G57">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2903,10 +4718,380 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>1024</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>22000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10">
+        <f>B8/(B8+B9)</f>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="9">
+        <f>B3*B8/(B9+B8)</f>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8">
+        <f>B12/B4*B$5</f>
+        <v>468.1142857142857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="10">
+        <f>(5/B$5)*(B9+B8)/B8</f>
+        <v>0.1025390625</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="12">
+        <f>B16*1023</f>
+        <v>104.8974609375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>1024</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>600</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <f>(50/(B3*B3))*600</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="10">
+        <f>(B11/50)*(B3*B3)/(B4*B4)</f>
+        <v>5.7220458984375E-4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16">
+        <f>50/B11</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>1024</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <f>(B8*B9)/1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="12">
+        <f>B5*1000/(B8*B9)</f>
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="10">
+        <f>(B5/B6)/B10</f>
+        <v>4.8828125E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,100 +5099,162 @@
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>256</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <f>60/1024</f>
-        <v>5.859375E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6">
+        <f>B5*voltage!B10</f>
+        <v>2.6190476190476191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="8">
+        <f>(B6/B1)*B2</f>
+        <v>134.0952380952381</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7">
-        <f>20/1024</f>
-        <v>1.953125E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
       <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B11">
-        <f>SQRT(50*B10)</f>
-        <v>223.60679774997897</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <f>B10*Current!B10</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13">
-        <f>200/1024</f>
-        <v>0.1953125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="B12">
+        <f>(B11/B1)*B2</f>
+        <v>112.64000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B16">
+        <f>SQRT(B15*'Fwd, Reverse power'!B16)</f>
+        <v>2.0412414523193148</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17">
-        <f>120/1024</f>
-        <v>0.1171875</v>
+        <v>67</v>
+      </c>
+      <c r="B17" s="8">
+        <f>(B16/B1)*B2</f>
+        <v>104.51156235874892</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20">
+        <v>600</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed current scaling and zero offset
</commit_message>
<xml_diff>
--- a/documentation/temp sensor calculator.xlsx
+++ b/documentation/temp sensor calculator.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>500W amplifier current sensing</t>
   </si>
@@ -255,9 +255,6 @@
     <t>Interpol</t>
   </si>
   <si>
-    <t>Hall effect sensor ACS723-40A</t>
-  </si>
-  <si>
     <t>-40A assumed!</t>
   </si>
   <si>
@@ -351,6 +348,27 @@
   </si>
   <si>
     <t>Full scale reading</t>
+  </si>
+  <si>
+    <t>Hall effect sensor</t>
+  </si>
+  <si>
+    <t>ACS723LLCTR-40AU-T</t>
+  </si>
+  <si>
+    <t>potential divider</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>divider factor</t>
+  </si>
+  <si>
+    <t>Also note these is a bias to null out.</t>
   </si>
 </sst>
 </file>
@@ -731,8 +749,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1617135856"/>
-        <c:axId val="-1617135312"/>
+        <c:axId val="443881536"/>
+        <c:axId val="443882080"/>
         <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -933,7 +951,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -1011,7 +1029,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$C$25:$C$45</c15:sqref>
@@ -1088,7 +1106,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -1113,7 +1131,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -1191,7 +1209,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$D$25:$D$45</c15:sqref>
@@ -1268,7 +1286,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -1279,7 +1297,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1617135856"/>
+        <c:axId val="443881536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1382,7 +1400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1617135312"/>
+        <c:crossAx val="443882080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1390,7 +1408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1617135312"/>
+        <c:axId val="443882080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1496,7 +1514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1617135856"/>
+        <c:crossAx val="443881536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1976,11 +1994,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1617127696"/>
-        <c:axId val="-1617134768"/>
+        <c:axId val="443868480"/>
+        <c:axId val="443869024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1617127696"/>
+        <c:axId val="443868480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2037,12 +2055,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1617134768"/>
+        <c:crossAx val="443869024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1617134768"/>
+        <c:axId val="443869024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -2101,7 +2119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1617127696"/>
+        <c:crossAx val="443868480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2115,7 +2133,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3321,7 +3338,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3371,7 +3388,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3421,7 +3438,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3471,7 +3488,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3521,7 +3538,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3557,7 +3574,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4799,14 +4816,14 @@
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10">
         <f>B8/(B8+B9)</f>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4869,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="12">
         <f>B16*1023</f>
@@ -4962,14 +4979,14 @@
     </row>
     <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16">
         <f>50/B11</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -4979,10 +4996,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4997,10 +5014,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5038,22 +5058,23 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <f>B19</f>
+        <v>0.66225165562913912</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <f>(B8*B9)/1000</f>
-        <v>0.1</v>
+        <v>6.6225165562913912E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -5062,7 +5083,7 @@
       </c>
       <c r="B11" s="12">
         <f>B5*1000/(B8*B9)</f>
-        <v>50</v>
+        <v>75.499999999999986</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
@@ -5070,14 +5091,55 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="10">
         <f>(B5/B6)/B10</f>
-        <v>4.8828125E-2</v>
+        <v>7.373046875E-2</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17">
+        <v>10000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18">
+        <v>5100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <f>B17/(B17+B18)</f>
+        <v>0.66225165562913912</v>
       </c>
     </row>
   </sheetData>
@@ -5101,7 +5163,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1">
         <v>5</v>
@@ -5110,18 +5172,18 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>256</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5131,7 +5193,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>55</v>
@@ -5142,7 +5204,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <f>B5*voltage!B10</f>
@@ -5154,7 +5216,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="8">
         <f>(B6/B1)*B2</f>
@@ -5168,7 +5230,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>22</v>
@@ -5179,11 +5241,11 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <f>B10*Current!B10</f>
-        <v>2.2000000000000002</v>
+        <v>1.4569536423841061</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -5191,21 +5253,21 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12">
         <f>(B11/B1)*B2</f>
-        <v>112.64000000000001</v>
+        <v>74.596026490066237</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -5216,7 +5278,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16">
         <f>SQRT(B15*'Fwd, Reverse power'!B16)</f>
@@ -5228,7 +5290,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="8">
         <f>(B16/B1)*B2</f>
@@ -5237,24 +5299,24 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20">
         <v>600</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21">
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update power display and current threshold
Current threshold = 27A
power display only rewrites if it has moved by more that 10W to reduce jitter
</commit_message>
<xml_diff>
--- a/documentation/temp sensor calculator.xlsx
+++ b/documentation/temp sensor calculator.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loz\SkyDrive\documents\amateur radio\SDR\ganymede\github\Ganymede\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\documents\amateur radio\SDR\ganymede\github\Ganymede\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2D6AE2-0128-46CB-AB89-D1C3D11DA948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="temp sensor" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Current" sheetId="5" r:id="rId4"/>
     <sheet name="comparator thresholds" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>500W amplifier current sensing</t>
   </si>
@@ -370,11 +371,26 @@
   <si>
     <t>Also note these is a bias to null out.</t>
   </si>
+  <si>
+    <t>ACS723 bias</t>
+  </si>
+  <si>
+    <t>bias at input to Ganymede</t>
+  </si>
+  <si>
+    <t>equivalent bias current</t>
+  </si>
+  <si>
+    <t>trip including bias</t>
+  </si>
+  <si>
+    <t>A apparent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -522,7 +538,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -734,7 +750,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-145C-464F-9456-78D9F4972EA5}"/>
             </c:ext>
@@ -749,9 +765,9 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="443881536"/>
-        <c:axId val="443882080"/>
-        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+        <c:axId val="-373321168"/>
+        <c:axId val="-373318992"/>
+        <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -771,7 +787,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -849,7 +865,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$B$25:$B$45</c15:sqref>
@@ -926,7 +942,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -951,7 +967,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -1029,7 +1045,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$C$25:$C$45</c15:sqref>
@@ -1106,7 +1122,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -1131,7 +1147,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -1209,7 +1225,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$D$25:$D$45</c15:sqref>
@@ -1286,7 +1302,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -1297,7 +1313,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="443881536"/>
+        <c:axId val="-373321168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443882080"/>
+        <c:crossAx val="-373318992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1408,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443882080"/>
+        <c:axId val="-373318992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,7 +1530,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443881536"/>
+        <c:crossAx val="-373321168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1595,7 +1611,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1863,7 +1879,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-3B35-43A7-9D2C-73572078976D}"/>
             </c:ext>
@@ -1980,7 +1996,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-3B35-43A7-9D2C-73572078976D}"/>
             </c:ext>
@@ -1994,11 +2010,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="443868480"/>
-        <c:axId val="443869024"/>
+        <c:axId val="-373329872"/>
+        <c:axId val="-373332592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="443868480"/>
+        <c:axId val="-373329872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2055,12 +2071,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443869024"/>
+        <c:crossAx val="-373332592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="443869024"/>
+        <c:axId val="-373332592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -2119,7 +2135,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443868480"/>
+        <c:crossAx val="-373329872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2164,14 +2180,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3338,7 +3354,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3388,7 +3404,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3438,7 +3454,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3488,7 +3504,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3538,7 +3554,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3574,7 +3590,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3857,74 +3873,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView topLeftCell="F44" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
       <selection activeCell="F51" sqref="F51:G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -3932,7 +3948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>18</v>
       </c>
@@ -3943,7 +3959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -3957,7 +3973,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>16</v>
       </c>
@@ -3968,7 +3984,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>35</v>
       </c>
@@ -3979,7 +3995,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -4002,7 +4018,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>-20</v>
       </c>
@@ -4018,7 +4034,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -4038,7 +4054,7 @@
         <v>79.645099959670446</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -4064,7 +4080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -4084,7 +4100,7 @@
         <v>123.47818319860657</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>15</v>
       </c>
@@ -4104,7 +4120,7 @@
         <v>150.93350802489357</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20</v>
       </c>
@@ -4130,7 +4146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>25</v>
       </c>
@@ -4150,7 +4166,7 @@
         <v>217.70078740157481</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4170,7 +4186,7 @@
         <v>256.47495361781074</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>35</v>
       </c>
@@ -4196,7 +4212,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>40</v>
       </c>
@@ -4216,7 +4232,7 @@
         <v>342.51734390485632</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>45</v>
       </c>
@@ -4236,7 +4252,7 @@
         <v>388.1238155401137</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>50</v>
       </c>
@@ -4262,7 +4278,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>55</v>
       </c>
@@ -4282,7 +4298,7 @@
         <v>481.73122157754432</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>60</v>
       </c>
@@ -4302,7 +4318,7 @@
         <v>528.04675413968948</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>65</v>
       </c>
@@ -4328,7 +4344,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>70</v>
       </c>
@@ -4348,7 +4364,7 @@
         <v>615.19291531307022</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>75</v>
       </c>
@@ -4368,7 +4384,7 @@
         <v>655.42991252400248</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>80</v>
       </c>
@@ -4394,7 +4410,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>85</v>
       </c>
@@ -4414,7 +4430,7 @@
         <v>727.54065575496031</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>90</v>
       </c>
@@ -4434,7 +4450,7 @@
         <v>759.1871030454804</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>95</v>
       </c>
@@ -4454,7 +4470,7 @@
         <v>787.92576717887925</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>100</v>
       </c>
@@ -4480,7 +4496,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>105</v>
       </c>
@@ -4500,7 +4516,7 @@
         <v>836.8114722591306</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>110</v>
       </c>
@@ -4520,7 +4536,7 @@
         <v>857.32093409779441</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>115</v>
       </c>
@@ -4540,7 +4556,7 @@
         <v>875.67660016532955</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>120</v>
       </c>
@@ -4560,7 +4576,7 @@
         <v>891.97742956417369</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>125</v>
       </c>
@@ -4586,7 +4602,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>130</v>
       </c>
@@ -4606,7 +4622,7 @@
         <v>919.01450585685598</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>135</v>
       </c>
@@ -4626,7 +4642,7 @@
         <v>930.30767988371156</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>140</v>
       </c>
@@ -4646,7 +4662,7 @@
         <v>940.29942115537654</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>145</v>
       </c>
@@ -4672,7 +4688,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>150</v>
       </c>
@@ -4692,7 +4708,7 @@
         <v>957.02590906730825</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>155</v>
       </c>
@@ -4712,7 +4728,7 @@
         <v>963.97304166826473</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>180</v>
       </c>
@@ -4734,27 +4750,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4765,7 +4781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -4776,7 +4792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -4787,12 +4803,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -4803,7 +4819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4814,7 +4830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>71</v>
       </c>
@@ -4826,7 +4842,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -4838,7 +4854,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -4847,15 +4863,15 @@
         <v>468.1142857142857</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="8"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -4867,7 +4883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -4883,24 +4899,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -4911,7 +4927,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4922,17 +4938,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4940,7 +4956,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -4951,7 +4967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4960,12 +4976,12 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -4977,7 +4993,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -4995,24 +5011,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -5023,7 +5039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5034,7 +5050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5045,7 +5061,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -5056,16 +5072,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
       <c r="B9">
-        <f>B19</f>
+        <f>B23</f>
         <v>0.66225165562913912</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -5077,7 +5093,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -5089,7 +5105,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -5101,44 +5117,79 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17">
+        <f>B16*B9</f>
+        <v>0.33112582781456956</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18">
+        <f>B17/B10</f>
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>83</v>
       </c>
-      <c r="B17">
+      <c r="B21">
         <v>10000</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>84</v>
       </c>
-      <c r="B18">
+      <c r="B22">
         <v>5100</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>85</v>
       </c>
-      <c r="B19">
-        <f>B17/(B17+B18)</f>
+      <c r="B23">
+        <f>B21/(B21+B22)</f>
         <v>0.66225165562913912</v>
       </c>
     </row>
@@ -5149,19 +5200,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -5175,7 +5226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -5186,12 +5237,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -5202,7 +5253,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -5214,7 +5265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -5223,99 +5274,111 @@
         <v>134.0952380952381</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
       <c r="B10">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <f>B10+Current!B18</f>
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>70</v>
       </c>
-      <c r="B11">
-        <f>B10*Current!B10</f>
-        <v>1.4569536423841061</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B12">
+        <f>B11*Current!B10</f>
+        <v>2.1192052980132452</v>
+      </c>
+      <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>66</v>
       </c>
-      <c r="B12">
-        <f>(B11/B1)*B2</f>
-        <v>74.596026490066237</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B13" s="8">
+        <f>(B12/B1)*B2</f>
+        <v>108.50331125827816</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>69</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>100</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>70</v>
       </c>
-      <c r="B16">
-        <f>SQRT(B15*'Fwd, Reverse power'!B16)</f>
+      <c r="B17">
+        <f>SQRT(B16*'Fwd, Reverse power'!B16)</f>
         <v>2.0412414523193148</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="8">
-        <f>(B16/B1)*B2</f>
+      <c r="B18" s="8">
+        <f>(B17/B1)*B2</f>
         <v>104.51156235874892</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>75</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>600</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change to bargraph displays for forward, reverse power
</commit_message>
<xml_diff>
--- a/documentation/temp sensor calculator.xlsx
+++ b/documentation/temp sensor calculator.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\documents\amateur radio\SDR\ganymede\github\Ganymede\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loz\SkyDrive\documents\amateur radio\SDR\ganymede\github\Ganymede\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2D6AE2-0128-46CB-AB89-D1C3D11DA948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="temp sensor" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Current" sheetId="5" r:id="rId4"/>
     <sheet name="comparator thresholds" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -390,7 +389,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -538,7 +537,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -750,7 +749,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-145C-464F-9456-78D9F4972EA5}"/>
             </c:ext>
@@ -765,9 +764,9 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-373321168"/>
-        <c:axId val="-373318992"/>
-        <c:extLst>
+        <c:axId val="-2083921536"/>
+        <c:axId val="-2083914464"/>
+        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -787,7 +786,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -865,7 +864,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$B$25:$B$45</c15:sqref>
@@ -942,7 +941,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -967,7 +966,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -1045,7 +1044,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$C$25:$C$45</c15:sqref>
@@ -1122,7 +1121,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -1147,7 +1146,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -1225,7 +1224,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$D$25:$D$45</c15:sqref>
@@ -1302,7 +1301,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -1313,7 +1312,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-373321168"/>
+        <c:axId val="-2083921536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,7 +1415,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-373318992"/>
+        <c:crossAx val="-2083914464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1424,7 +1423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-373318992"/>
+        <c:axId val="-2083914464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1530,7 +1529,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-373321168"/>
+        <c:crossAx val="-2083921536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1611,7 +1610,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1879,7 +1878,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-3B35-43A7-9D2C-73572078976D}"/>
             </c:ext>
@@ -1996,7 +1995,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-3B35-43A7-9D2C-73572078976D}"/>
             </c:ext>
@@ -2010,11 +2009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-373329872"/>
-        <c:axId val="-373332592"/>
+        <c:axId val="-2083913920"/>
+        <c:axId val="-2083909024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-373329872"/>
+        <c:axId val="-2083913920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2071,12 +2070,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-373332592"/>
+        <c:crossAx val="-2083909024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-373332592"/>
+        <c:axId val="-2083909024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -2135,7 +2134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-373329872"/>
+        <c:crossAx val="-2083913920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2180,14 +2179,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3354,7 +3353,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3404,7 +3403,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3454,7 +3453,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3504,7 +3503,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3554,7 +3553,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3590,7 +3589,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3873,74 +3872,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView topLeftCell="F44" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
       <selection activeCell="F51" sqref="F51:G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -3948,7 +3947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>18</v>
       </c>
@@ -3959,7 +3958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -3973,7 +3972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>16</v>
       </c>
@@ -3984,7 +3983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>35</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -4018,7 +4017,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-20</v>
       </c>
@@ -4034,7 +4033,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>79.645099959670446</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -4080,7 +4079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -4100,7 +4099,7 @@
         <v>123.47818319860657</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15</v>
       </c>
@@ -4120,7 +4119,7 @@
         <v>150.93350802489357</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
@@ -4146,7 +4145,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>25</v>
       </c>
@@ -4166,7 +4165,7 @@
         <v>217.70078740157481</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4186,7 +4185,7 @@
         <v>256.47495361781074</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>35</v>
       </c>
@@ -4212,7 +4211,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>40</v>
       </c>
@@ -4232,7 +4231,7 @@
         <v>342.51734390485632</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>45</v>
       </c>
@@ -4252,7 +4251,7 @@
         <v>388.1238155401137</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>50</v>
       </c>
@@ -4278,7 +4277,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>55</v>
       </c>
@@ -4298,7 +4297,7 @@
         <v>481.73122157754432</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>60</v>
       </c>
@@ -4318,7 +4317,7 @@
         <v>528.04675413968948</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>65</v>
       </c>
@@ -4344,7 +4343,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>70</v>
       </c>
@@ -4364,7 +4363,7 @@
         <v>615.19291531307022</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>75</v>
       </c>
@@ -4384,7 +4383,7 @@
         <v>655.42991252400248</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>80</v>
       </c>
@@ -4410,7 +4409,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>85</v>
       </c>
@@ -4430,7 +4429,7 @@
         <v>727.54065575496031</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>90</v>
       </c>
@@ -4450,7 +4449,7 @@
         <v>759.1871030454804</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>95</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>787.92576717887925</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>100</v>
       </c>
@@ -4496,7 +4495,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>105</v>
       </c>
@@ -4516,7 +4515,7 @@
         <v>836.8114722591306</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>110</v>
       </c>
@@ -4536,7 +4535,7 @@
         <v>857.32093409779441</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>115</v>
       </c>
@@ -4556,7 +4555,7 @@
         <v>875.67660016532955</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>120</v>
       </c>
@@ -4576,7 +4575,7 @@
         <v>891.97742956417369</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>125</v>
       </c>
@@ -4602,7 +4601,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>130</v>
       </c>
@@ -4622,7 +4621,7 @@
         <v>919.01450585685598</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>135</v>
       </c>
@@ -4642,7 +4641,7 @@
         <v>930.30767988371156</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>140</v>
       </c>
@@ -4662,7 +4661,7 @@
         <v>940.29942115537654</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>145</v>
       </c>
@@ -4688,7 +4687,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>150</v>
       </c>
@@ -4708,7 +4707,7 @@
         <v>957.02590906730825</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>155</v>
       </c>
@@ -4728,7 +4727,7 @@
         <v>963.97304166826473</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>180</v>
       </c>
@@ -4750,27 +4749,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4781,7 +4780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -4792,7 +4791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -4803,12 +4802,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -4819,7 +4818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>71</v>
       </c>
@@ -4842,7 +4841,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -4854,7 +4853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -4863,15 +4862,15 @@
         <v>468.1142857142857</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -4883,7 +4882,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -4899,24 +4898,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -4927,7 +4926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4938,17 +4937,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4956,7 +4955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -4967,7 +4966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4976,12 +4975,12 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -4993,7 +4992,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -5011,24 +5010,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -5039,7 +5038,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5050,7 +5049,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5061,7 +5060,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -5072,7 +5071,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -5081,7 +5080,7 @@
         <v>0.66225165562913912</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -5093,7 +5092,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -5105,7 +5104,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -5117,12 +5116,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -5133,7 +5132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -5145,7 +5144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -5157,12 +5156,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -5173,7 +5172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -5184,7 +5183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -5200,19 +5199,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -5226,7 +5225,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -5237,12 +5236,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -5253,7 +5252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -5265,7 +5264,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -5274,61 +5273,61 @@
         <v>134.0952380952381</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
       <c r="B10">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
       <c r="B11">
         <f>B10+Current!B18</f>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
       <c r="B12">
         <f>B11*Current!B10</f>
-        <v>2.1192052980132452</v>
+        <v>2.4503311258278146</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
       <c r="B13" s="8">
         <f>(B12/B1)*B2</f>
-        <v>108.50331125827816</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>125.45695364238411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -5339,7 +5338,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -5351,7 +5350,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -5360,7 +5359,7 @@
         <v>104.51156235874892</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -5371,7 +5370,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
updates for G2-1K including engineering page
</commit_message>
<xml_diff>
--- a/documentation/temp sensor calculator.xlsx
+++ b/documentation/temp sensor calculator.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loz\SkyDrive\documents\amateur radio\SDR\ganymede\github\Ganymede\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d529807eb1393ed/documents/amateur radio/SDR/ganymede/github/Ganymede/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="440" documentId="11_0B940810EFE5780F5203872B4B013B0D3336DB44" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C676AF0C-6548-4F3B-A8DF-6223E2784F5C}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="4"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="temp sensor" sheetId="1" r:id="rId1"/>
     <sheet name="voltage" sheetId="3" r:id="rId2"/>
     <sheet name="Fwd, Reverse power" sheetId="4" r:id="rId3"/>
     <sheet name="Current" sheetId="5" r:id="rId4"/>
-    <sheet name="comparator thresholds" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +29,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="118">
   <si>
     <t>500W amplifier current sensing</t>
   </si>
@@ -111,33 +114,12 @@
     <t>ADC</t>
   </si>
   <si>
-    <t>voltage</t>
-  </si>
-  <si>
-    <t>current</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
-    <t>Input voltage</t>
-  </si>
-  <si>
-    <t>sensor voltage</t>
-  </si>
-  <si>
     <t>AREF</t>
   </si>
   <si>
-    <t>ADC reading</t>
-  </si>
-  <si>
-    <t>R34</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
     <t>Divider on pallet PCB:</t>
   </si>
   <si>
@@ -168,81 +150,12 @@
     <t>Full scale voltage</t>
   </si>
   <si>
-    <t>R49, R50 on divider adjusted to give 5V for input power &gt; 500W</t>
-  </si>
-  <si>
-    <t>Full power calibrated value</t>
-  </si>
-  <si>
-    <t>we don't know the calibration of the VSWR bridge exactly</t>
-  </si>
-  <si>
-    <r>
-      <t>power = K. V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/R</t>
-    </r>
-  </si>
-  <si>
-    <t>R=50 ohms</t>
-  </si>
-  <si>
-    <t>K=</t>
-  </si>
-  <si>
-    <t>Calibration for power from ADC value:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power (W) = </t>
-  </si>
-  <si>
-    <r>
-      <t>* ADC reading</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
     <t>Current Sensor</t>
   </si>
   <si>
     <t>Output voltage scale</t>
   </si>
   <si>
-    <t>mV/A</t>
-  </si>
-  <si>
-    <t>full scale current</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -255,146 +168,256 @@
     <t>Interpol</t>
   </si>
   <si>
-    <t>-40A assumed!</t>
-  </si>
-  <si>
-    <t>sensor circuit gain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anode current (A) = </t>
-  </si>
-  <si>
-    <t>effective scale</t>
-  </si>
-  <si>
     <t>V/A</t>
   </si>
   <si>
-    <t>DAC output level</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>DAC full scale count</t>
-  </si>
-  <si>
-    <t>(8 bits)</t>
-  </si>
-  <si>
-    <t>trip voltage</t>
-  </si>
-  <si>
-    <t>DAC setting</t>
-  </si>
-  <si>
-    <t>trip current</t>
-  </si>
-  <si>
-    <t>reverse power</t>
-  </si>
-  <si>
-    <t>trip power</t>
-  </si>
-  <si>
-    <t>comparator voltage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensor &amp; comparator input = </t>
-  </si>
-  <si>
     <t>*input voltage</t>
   </si>
   <si>
-    <t>*power</t>
-  </si>
-  <si>
-    <r>
-      <t>V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <t>Forward power trip</t>
-  </si>
-  <si>
-    <t>temperature trip</t>
-  </si>
-  <si>
-    <t>C (software)</t>
-  </si>
-  <si>
-    <t>W (software)</t>
-  </si>
-  <si>
     <t>Full scale reading</t>
   </si>
   <si>
     <t>Hall effect sensor</t>
   </si>
   <si>
+    <t>R111</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>Forward power</t>
+  </si>
+  <si>
+    <t>Reverse power</t>
+  </si>
+  <si>
+    <t>transformer coupling turns</t>
+  </si>
+  <si>
+    <t>dB</t>
+  </si>
+  <si>
+    <t>R4, R10-R12</t>
+  </si>
+  <si>
+    <t>R3, R6, R7</t>
+  </si>
+  <si>
+    <t>RF volts RMS</t>
+  </si>
+  <si>
+    <t>Sensed path</t>
+  </si>
+  <si>
+    <t>R113</t>
+  </si>
+  <si>
+    <t>R112</t>
+  </si>
+  <si>
+    <t>R114</t>
+  </si>
+  <si>
+    <t>potentiometer</t>
+  </si>
+  <si>
+    <t>division ratio</t>
+  </si>
+  <si>
+    <t>(insignificant)</t>
+  </si>
+  <si>
+    <t>potentiometer aimpoint</t>
+  </si>
+  <si>
+    <t>combined division ratio to potentiometer</t>
+  </si>
+  <si>
+    <t>(aim for 3.5)</t>
+  </si>
+  <si>
+    <t>voltage follower (U5B) output</t>
+  </si>
+  <si>
+    <t>final potential divider (R114, potentiometer)</t>
+  </si>
+  <si>
+    <t>sensor &amp; ADC input scaling</t>
+  </si>
+  <si>
+    <t>At trip voltage:</t>
+  </si>
+  <si>
+    <t>Input voltage at trip point</t>
+  </si>
+  <si>
+    <t>sensor  &amp; ADC voltage</t>
+  </si>
+  <si>
     <t>ACS723LLCTR-40AU-T</t>
   </si>
   <si>
-    <t>potential divider</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>divider factor</t>
-  </si>
-  <si>
-    <t>Also note these is a bias to null out.</t>
-  </si>
-  <si>
-    <t>ACS723 bias</t>
-  </si>
-  <si>
-    <t>bias at input to Ganymede</t>
-  </si>
-  <si>
-    <t>equivalent bias current</t>
-  </si>
-  <si>
-    <t>trip including bias</t>
-  </si>
-  <si>
-    <t>A apparent</t>
+    <t>(from current sensor datasheet)</t>
+  </si>
+  <si>
+    <t>sensor circuit potential divider R109, R111</t>
+  </si>
+  <si>
+    <t>voltage follower (U5A) output</t>
+  </si>
+  <si>
+    <t>final potential divider (R110, potentiometer)</t>
+  </si>
+  <si>
+    <t>R110</t>
+  </si>
+  <si>
+    <t>*PA current</t>
+  </si>
+  <si>
+    <t>Trip current</t>
+  </si>
+  <si>
+    <t>(aim for 3.5V)</t>
+  </si>
+  <si>
+    <t>(derived from current sensor datasheet)</t>
+  </si>
+  <si>
+    <t>sensor &amp; ADC input voltage at trip current</t>
+  </si>
+  <si>
+    <t>ADC reading at trip current</t>
+  </si>
+  <si>
+    <t>ADC reading at trip voltage</t>
+  </si>
+  <si>
+    <t>(user to derive software constants)</t>
+  </si>
+  <si>
+    <t>scaling factor to convert ADC reading to PA current:</t>
+  </si>
+  <si>
+    <t>PA current  =</t>
+  </si>
+  <si>
+    <t>Full scale current reading</t>
+  </si>
+  <si>
+    <t>Some current sensors have a bias current, to allow reading of small negative currents</t>
+  </si>
+  <si>
+    <t>For these: measure ADC voltage when there is no current present; subtract from ADC readings to get true PA current.</t>
+  </si>
+  <si>
+    <t>Offset current (derived from sensor output voltage @ 0A)</t>
+  </si>
+  <si>
+    <t>* (ADC reading - ADC reading with PA off)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potentiometers R65, R66 on control board adjusted to set analogue in to Arduino </t>
+  </si>
+  <si>
+    <t>R2, R5 on LPF board to be omitted (not needed, and would only make sense if midpoint was grounded)</t>
+  </si>
+  <si>
+    <t>max power at trip point</t>
+  </si>
+  <si>
+    <t>(reverse power assumes trip at 3:1 VSWR)</t>
+  </si>
+  <si>
+    <t>transformer division (linear volts)</t>
+  </si>
+  <si>
+    <t>resistive pad after VSWR bridge, still 50Ω RF</t>
+  </si>
+  <si>
+    <t>resistor Pad resistors</t>
+  </si>
+  <si>
+    <t>resistive pad volt drop</t>
+  </si>
+  <si>
+    <t>potential divider with R8/R9 &amp; 10K pot:</t>
+  </si>
+  <si>
+    <t>R8/R9 value</t>
+  </si>
+  <si>
+    <t>potentiometer value</t>
+  </si>
+  <si>
+    <t>peak voltage across potentiometer at trip</t>
+  </si>
+  <si>
+    <t>potentiometer setting</t>
+  </si>
+  <si>
+    <t>ADC, comparator input at trip point</t>
+  </si>
+  <si>
+    <t>RF volts peak</t>
+  </si>
+  <si>
+    <t>peak voltage at VSWR bridge output</t>
+  </si>
+  <si>
+    <t>the original 30 &amp; 20 dB much too big!</t>
+  </si>
+  <si>
+    <t>total division ratio to ADC, comparator</t>
+  </si>
+  <si>
+    <t>combined division ratio to get voltage across potentiometer</t>
+  </si>
+  <si>
+    <t>scaling factor to convert ADC reading to RF voltage &amp; power:</t>
+  </si>
+  <si>
+    <t>ADC reading at trip point</t>
+  </si>
+  <si>
+    <t>RMS RF voltage (Volts) =</t>
+  </si>
+  <si>
+    <t>Full scale reading (RMS volts)</t>
+  </si>
+  <si>
+    <t>full scale power</t>
+  </si>
+  <si>
+    <t>to get 6dB pads: shunt R=150, series R=39</t>
+  </si>
+  <si>
+    <t>comparator PWM setting</t>
+  </si>
+  <si>
+    <t>current PWM setting</t>
+  </si>
+  <si>
+    <t>comparator PWM setting for reverse power</t>
+  </si>
+  <si>
+    <t>scale factor to watts</t>
+  </si>
+  <si>
+    <t>* ADC reading squared</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,12 +457,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -496,10 +530,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -518,10 +553,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -537,7 +586,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -749,7 +798,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-145C-464F-9456-78D9F4972EA5}"/>
             </c:ext>
@@ -766,7 +815,7 @@
         <c:smooth val="0"/>
         <c:axId val="-2083921536"/>
         <c:axId val="-2083914464"/>
-        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+        <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -786,7 +835,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -864,7 +913,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$B$25:$B$45</c15:sqref>
@@ -941,7 +990,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -966,7 +1015,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -1044,7 +1093,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$C$25:$C$45</c15:sqref>
@@ -1121,7 +1170,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -1146,7 +1195,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$A$25:$A$45</c15:sqref>
@@ -1224,7 +1273,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'temp sensor'!$D$25:$D$45</c15:sqref>
@@ -1301,7 +1350,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-145C-464F-9456-78D9F4972EA5}"/>
                   </c:ext>
@@ -1374,7 +1423,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-GB"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1610,7 +1659,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1878,7 +1927,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-3B35-43A7-9D2C-73572078976D}"/>
             </c:ext>
@@ -1995,7 +2044,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-3B35-43A7-9D2C-73572078976D}"/>
             </c:ext>
@@ -2180,7 +2229,7 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
     <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
@@ -3353,7 +3402,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3403,7 +3452,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3453,7 +3502,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3503,7 +3552,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3553,7 +3602,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3589,7 +3638,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B089EC-CD7F-47B8-B627-D5A64C024BB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3872,10 +3921,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="F44" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
       <selection activeCell="F51" sqref="F51:G51"/>
     </sheetView>
   </sheetViews>
@@ -3985,13 +4034,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E21">
         <v>1024</v>
       </c>
       <c r="F21" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -4014,7 +4063,7 @@
         <v>19</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -4749,40 +4798,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -4791,104 +4840,197 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>1024</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B8">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B9">
-        <v>22000</v>
+        <v>13000</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B10">
         <f>B8/(B8+B9)</f>
-        <v>4.7619047619047616E-2</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>10000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <f>B13/(B13+B12)</f>
+        <v>0.99532198666268534</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <f>B10*B14</f>
+        <v>7.1094427618763237E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="17">
+        <f>B15*B16</f>
+        <v>6.3984984856886917E-2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="9">
+        <f>B3*B10*B14*B16</f>
+        <v>3.3912041974150062</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="8">
+        <f>B20/B4*B$5</f>
+        <v>694.51861963059332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="8">
+        <f>256*(B20/B4)</f>
+        <v>173.62965490764833</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="9">
-        <f>B3*B8/(B9+B8)</f>
-        <v>2.2857142857142856</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B26" s="10">
+        <f>(B$4/B$5)*(1/B17)</f>
+        <v>7.6311848958333331E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="12">
+        <f>B26*1023</f>
+        <v>78.067021484375005</v>
+      </c>
+      <c r="C28" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="8">
-        <f>B12/B4*B$5</f>
-        <v>468.1142857142857</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="10">
-        <f>(5/B$5)*(B9+B8)/B8</f>
-        <v>0.1025390625</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="12">
-        <f>B16*1023</f>
-        <v>104.8974609375</v>
       </c>
     </row>
   </sheetData>
@@ -4898,26 +5040,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="46.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -4926,121 +5070,418 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>1024</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10">
-        <v>600</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1500</v>
+      </c>
+      <c r="C10" s="13">
+        <f>B10/4</f>
+        <v>375</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11">
-        <f>(50/(B3*B3))*600</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="B11" s="12">
+        <f>SQRT(B10*50)</f>
+        <v>273.86127875258308</v>
+      </c>
+      <c r="C11" s="12">
+        <f>SQRT(C10*50)</f>
+        <v>136.93063937629154</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="21">
+        <f>SQRT(2)*B11</f>
+        <v>387.29833462074174</v>
+      </c>
+      <c r="C12" s="21">
+        <f>SQRT(2)*C11</f>
+        <v>193.64916731037087</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="10">
-        <f>(B11/50)*(B3*B3)/(B4*B4)</f>
-        <v>5.7220458984375E-4</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15">
+        <f>1/B14</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C15">
+        <f>1/C14</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="7">
+        <f>B12*B15</f>
+        <v>16.137430609197573</v>
+      </c>
+      <c r="C16" s="7">
+        <f>C12*C15</f>
+        <v>8.0687153045987863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16">
-        <f>50/B11</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>73</v>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20">
+        <f>1/(10^(B18/20))</f>
+        <v>0.25118864315095801</v>
+      </c>
+      <c r="C20">
+        <f>1/(10^(C18/20))</f>
+        <v>0.50118723362727224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22">
+        <v>510</v>
+      </c>
+      <c r="C22">
+        <v>510</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23">
+        <v>10000</v>
+      </c>
+      <c r="C23">
+        <v>10000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24">
+        <f>B23/(B23+B22)</f>
+        <v>0.95147478591817314</v>
+      </c>
+      <c r="C24">
+        <f>C23/(C23+C22)</f>
+        <v>0.95147478591817314</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26">
+        <f>B15*B20*B24</f>
+        <v>9.9583191861305903E-3</v>
+      </c>
+      <c r="C26">
+        <f>C15*C20*C24</f>
+        <v>1.9869458992517929E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27">
+        <f>B12*B26</f>
+        <v>3.8568404364101578</v>
+      </c>
+      <c r="C27">
+        <f>C12*C26</f>
+        <v>3.8477041888086574</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="C29" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="14">
+        <f>B26*B29</f>
+        <v>8.9624872675175323E-3</v>
+      </c>
+      <c r="C30" s="14">
+        <f>C26*C29</f>
+        <v>1.7882513093266137E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31">
+        <f>B27*B29</f>
+        <v>3.4711563927691422</v>
+      </c>
+      <c r="C31">
+        <f>C27*C29</f>
+        <v>3.4629337699277918</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="8">
+        <f>($B4/$B3)*B31</f>
+        <v>710.89282923912037</v>
+      </c>
+      <c r="C32" s="8">
+        <f>($B4/$B3)*C31</f>
+        <v>709.20883608121176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8">
+        <f>256*(C31/B3)</f>
+        <v>177.30220902030294</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="10">
+        <f>($B$3/$B$4)*(1/B30)/SQRT(2)</f>
+        <v>0.38523567475803783</v>
+      </c>
+      <c r="C37" s="10">
+        <f>($B$3/$B$4)*(1/C30)/SQRT(2)</f>
+        <v>0.1930752021265166</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38">
+        <f>B37*B37/50</f>
+        <v>2.9681305021256139E-3</v>
+      </c>
+      <c r="C38">
+        <f>C37*C37/50</f>
+        <v>7.4556067352390476E-4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="12">
+        <f>B37*1023</f>
+        <v>394.09609527747267</v>
+      </c>
+      <c r="C40" s="12">
+        <f>C37*1023</f>
+        <v>197.51593177542648</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="8">
+        <f>B40*B40/50</f>
+        <v>3106.2346462590167</v>
+      </c>
+      <c r="C41" s="8">
+        <f>C40*C40/50</f>
+        <v>780.25086610229857</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="A1" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>53</v>
+      <c r="A5" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -5050,339 +5491,274 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>54</v>
+      <c r="A6" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="B6">
         <v>1024</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>49</v>
+      <c r="A8" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="10">
+        <v>2700</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>10000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <f>B8*B12/(B11+B12)</f>
+        <v>7.874015748031496E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17">
+        <v>10000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <f>B17/(B17+B16)</f>
+        <v>0.99532198666268534</v>
+      </c>
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="B9">
-        <f>B23</f>
-        <v>0.66225165562913912</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B10">
-        <f>(B8*B9)/1000</f>
-        <v>6.6225165562913912E-2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="12">
-        <f>B5*1000/(B8*B9)</f>
-        <v>75.499999999999986</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B19">
+        <f>B13*B18</f>
+        <v>7.8371809973439788E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="10">
-        <f>(B5/B6)/B10</f>
-        <v>7.373046875E-2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B20" s="16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="17">
+        <f>B19*B20</f>
+        <v>7.0534628976095817E-2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="19">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="17">
+        <f>(B23+B9)*B21</f>
+        <v>3.174058303924312</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="19">
+        <f>(B6/B5)*B24</f>
+        <v>650.04714064369909</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="19">
+        <f>256*(B24/B5)</f>
+        <v>162.51178516092477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="10">
+        <f>(B$5/B$6)*(1/B21)</f>
+        <v>6.9225748697916673E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30">
+        <f>B30*650</f>
+        <v>44.99673665364584</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="12">
+        <f>B30*1023</f>
+        <v>70.817940917968755</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="17"/>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="17"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="17"/>
+    </row>
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="17"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="10">
+        <f>B30</f>
+        <v>6.9225748697916673E-2</v>
+      </c>
+      <c r="C37" t="s">
         <v>87</v>
       </c>
-      <c r="B16">
-        <v>0.5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17">
-        <f>B16*B9</f>
-        <v>0.33112582781456956</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18">
-        <f>B17/B10</f>
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21">
-        <v>10000</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22">
-        <v>5100</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23">
-        <f>B21/(B21+B22)</f>
-        <v>0.66225165562913912</v>
-      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="12"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2">
-        <v>256</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6">
-        <f>B5*voltage!B10</f>
-        <v>2.6190476190476191</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="8">
-        <f>(B6/B1)*B2</f>
-        <v>134.0952380952381</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11">
-        <f>B10+Current!B18</f>
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12">
-        <f>B11*Current!B10</f>
-        <v>2.4503311258278146</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="8">
-        <f>(B12/B1)*B2</f>
-        <v>125.45695364238411</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16">
-        <v>100</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17">
-        <f>SQRT(B16*'Fwd, Reverse power'!B16)</f>
-        <v>2.0412414523193148</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="8">
-        <f>(B17/B1)*B2</f>
-        <v>104.51156235874892</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21">
-        <v>600</v>
-      </c>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22">
-        <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>